<commit_message>
do multiple table on 1 sheet
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/DataTest.xlsx
+++ b/src/main/resources/testdata/DataTest.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="NewAccountTest" sheetId="1" r:id="rId1"/>
-    <sheet name="NewAccountTest2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="EditAccountTest" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="37">
   <si>
     <t>Customer ID is required</t>
   </si>
@@ -91,6 +91,42 @@
   </si>
   <si>
     <t>Pass</t>
+  </si>
+  <si>
+    <t>EA1</t>
+  </si>
+  <si>
+    <t>Account Number must not be blank</t>
+  </si>
+  <si>
+    <t>EA2</t>
+  </si>
+  <si>
+    <t>expectedMessage</t>
+  </si>
+  <si>
+    <t>EA3</t>
+  </si>
+  <si>
+    <t>inputValue1</t>
+  </si>
+  <si>
+    <t>123@#</t>
+  </si>
+  <si>
+    <t>123@#!1</t>
+  </si>
+  <si>
+    <t>EA5</t>
+  </si>
+  <si>
+    <t>145 3</t>
+  </si>
+  <si>
+    <t>EA6</t>
+  </si>
+  <si>
+    <t>1 2</t>
   </si>
 </sst>
 </file>
@@ -116,15 +152,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -132,14 +174,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -583,7 +643,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -648,12 +708,174 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="3"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B8" r:id="rId1"/>
+    <hyperlink ref="C8" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>